<commit_message>
Końcowe wyniki wyzarzanie w tabeli
</commit_message>
<xml_diff>
--- a/wyniki_wyzarzanie/Wyniki_wyzarzanie_tabela.xlsx
+++ b/wyniki_wyzarzanie/Wyniki_wyzarzanie_tabela.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zimak\source\repos\ComputationalInteligence\wyniki_wyzarzanie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8A83FF-564F-4E59-84AB-6AA1764071FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D554C280-D0E3-4E52-AC2C-1206C02ED850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{01E9C1F5-D514-49A6-9A73-7E0CF90B0B32}"/>
   </bookViews>
@@ -1366,7 +1366,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1469,10 +1469,18 @@
       <c r="B5">
         <v>100</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="C5">
+        <v>118532.858643336</v>
+      </c>
+      <c r="D5">
+        <v>121139.51</v>
+      </c>
+      <c r="E5" s="4">
+        <v>6856.91</v>
+      </c>
       <c r="F5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>114.28183333333332</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1793,7 +1801,7 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F21" s="3">
         <f>SUM(F2:F20)</f>
-        <v>278.56283333333329</v>
+        <v>392.84466666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>